<commit_message>
Kin Insurance Coding Challenge
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Computer Science, Information &amp; General Works</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Arts &amp; Recreation</t>
+  </si>
+  <si>
+    <t>Total Pages Read</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -172,6 +175,14 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1402.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>